<commit_message>
Corregir variable VALOR_LETRAS para que coincida con el Excel template
</commit_message>
<xml_diff>
--- a/CONTRATO EXCEL FLORE JUNCALITO.xlsx
+++ b/CONTRATO EXCEL FLORE JUNCALITO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gm714\OneDrive\Escritorio\sistema_gestion_personal\templates_contratos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gm714\OneDrive\Escritorio\sistema_gestion_nuevo\templates_contratos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEEA281-FC3D-4657-91FE-28D73605F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD5F6AE-38FF-491C-8806-9431F5D6647A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t xml:space="preserve">  CONTRATO INDIVIDUAL DE TRABAJO POR LA LABOR CONTRATADA </t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>{CARGO_EMPLEADO}</t>
+  </si>
+  <si>
+    <t>{VALOR_LETRAS}</t>
   </si>
 </sst>
 </file>
@@ -375,37 +378,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -915,7 +918,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,11 +929,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -938,46 +941,46 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1011,61 +1014,60 @@
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13" t="str">
-        <f>C14</f>
-        <v>{CIUDAD_CONTRATACION}</v>
+      <c r="C10" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="18" t="s">
         <v>19</v>
       </c>
@@ -1076,196 +1078,196 @@
       <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
     </row>
     <row r="54" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
     </row>
     <row r="55" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
@@ -1344,12 +1346,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A18:C55"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
@@ -1357,6 +1353,12 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>